<commit_message>
Programa funcionando correctamente con extras de texto y parrafo
</commit_message>
<xml_diff>
--- a/pruebas.xlsx
+++ b/pruebas.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -407,24 +407,9 @@
         <v>573104023154</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>573215996243</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>573165021509</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>573164602901</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
envio constante sin guardar el ultimo envio funcionando
</commit_message>
<xml_diff>
--- a/pruebas.xlsx
+++ b/pruebas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farud\OneDrive\Escritorio\MGS_Selenium\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\MGS_Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879E31CE-8F69-4719-86A4-E34673693F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40BE59E-9936-4A3A-84FD-3E74BA3309A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,7 +394,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
funcionando correctamente, falta pulir
</commit_message>
<xml_diff>
--- a/pruebas.xlsx
+++ b/pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\MGS_Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40BE59E-9936-4A3A-84FD-3E74BA3309A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839B7F66-5D16-4F24-A7D7-8E63DD2F9DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -422,6 +422,26 @@
         <v>3215996243</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3215996243</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
un poco ordenado nuevo2.py
</commit_message>
<xml_diff>
--- a/pruebas.xlsx
+++ b/pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\MGS_Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839B7F66-5D16-4F24-A7D7-8E63DD2F9DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26010DC-4572-49AF-8294-9539FE1724AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A320"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A8"/>
+    <sheetView tabSelected="1" topLeftCell="A296" workbookViewId="0">
+      <selection activeCell="H306" sqref="H306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -429,17 +429,1577 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>3247439861</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>3104023154</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>3215996243</v>
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A164">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A165">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A167">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A168">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A173">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A174">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A175">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A176">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A177">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A178">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A179">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A180">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A181">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A182">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A183">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A184">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A185">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A186">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A187">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A188">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A189">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A190">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A191">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A192">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A193">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A194">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A195">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A196">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A197">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A198">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A199">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A200">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A201">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A202">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A203">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A204">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A205">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A206">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A207">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A208">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A209">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A210">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A211">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A212">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A213">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A214">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A215">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A216">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A217">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A218">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A219">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A220">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A221">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A222">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A223">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A224">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A225">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A226">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A227">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A228">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A229">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A230">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A231">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A232">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A233">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A234">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A235">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A236">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A237">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A238">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A239">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A240">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A241">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A242">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A243">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A244">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A245">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A246">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A247">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A248">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A249">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A250">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A251">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A252">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A253">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A254">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A255">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A256">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A257">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A258">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A259">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A260">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A261">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A262">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A263">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A264">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A265">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A266">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A267">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A268">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A269">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A270">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A271">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A272">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A273">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A274">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A275">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A276">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A277">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A278">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A279">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A280">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A281">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A282">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A283">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A284">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A285">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A286">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A287">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A288">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A289">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A290">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A291">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A292">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A293">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A294">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A295">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A296">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A297">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A298">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A299">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A300">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A301">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A302">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A303">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A304">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A305">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A306">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A307">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A308">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A309">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A310">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A311">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A312">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A313">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A314">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A315">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A316">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A317">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A318">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A319">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A320">
+        <v>3174466432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Funcionando cookies, y reinicio
</commit_message>
<xml_diff>
--- a/pruebas.xlsx
+++ b/pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\MGS_Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26010DC-4572-49AF-8294-9539FE1724AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC90080-5858-4550-8C7A-F6721BFC20FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -393,8 +393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A296" workbookViewId="0">
-      <selection activeCell="H306" sqref="H306"/>
+    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
+      <selection activeCell="A320" sqref="A320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -424,32 +424,32 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
@@ -474,32 +474,32 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
@@ -524,32 +524,32 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
@@ -574,32 +574,32 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
@@ -624,32 +624,32 @@
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
@@ -674,32 +674,32 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
@@ -724,32 +724,32 @@
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
@@ -774,32 +774,32 @@
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
@@ -824,32 +824,32 @@
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
@@ -874,32 +874,32 @@
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
@@ -924,32 +924,32 @@
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
@@ -974,32 +974,32 @@
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
@@ -1024,32 +1024,32 @@
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
@@ -1074,32 +1074,32 @@
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
@@ -1124,32 +1124,32 @@
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
@@ -1174,32 +1174,32 @@
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.3">
@@ -1224,32 +1224,32 @@
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.3">
@@ -1274,32 +1274,32 @@
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.3">
@@ -1324,32 +1324,32 @@
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.3">
@@ -1374,32 +1374,32 @@
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.3">
@@ -1424,32 +1424,32 @@
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A210">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.3">
@@ -1474,32 +1474,32 @@
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.3">
@@ -1524,32 +1524,32 @@
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.3">
@@ -1574,32 +1574,32 @@
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A237">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A239">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A240">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.3">
@@ -1624,32 +1624,32 @@
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A247">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A248">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A249">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.3">
@@ -1674,32 +1674,32 @@
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A255">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A256">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A257">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A258">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A259">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A260">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.3">
@@ -1724,32 +1724,32 @@
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A265">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A266">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A267">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A268">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A269">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A270">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.3">
@@ -1774,32 +1774,32 @@
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A275">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A276">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A277">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A278">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A279">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A280">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.3">
@@ -1824,32 +1824,32 @@
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A285">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A286">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A287">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A288">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A289">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A290">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.3">
@@ -1874,32 +1874,32 @@
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A295">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A296">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A298">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A299">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A300">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.3">
@@ -1924,32 +1924,32 @@
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A305">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A306">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A307">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A308">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A309">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A310">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.3">
@@ -1974,32 +1974,32 @@
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A315">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A316">
-        <v>3174466432</v>
+        <v>3176652286</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A317">
-        <v>3247439861</v>
+        <v>3173506184</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A318">
-        <v>3104023154</v>
+        <v>3172486789</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A319">
-        <v>3215996243</v>
+        <v>3173809096</v>
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A320">
-        <v>3174466432</v>
+        <v>3123144985</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizacion de tiempo varibale finalimeSleep.py
</commit_message>
<xml_diff>
--- a/pruebas.xlsx
+++ b/pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\MGS_Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC90080-5858-4550-8C7A-F6721BFC20FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768FE24B-869D-4C25-A941-82F103AC7E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A320"/>
+  <dimension ref="A1:A336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
-      <selection activeCell="A320" sqref="A320"/>
+    <sheetView tabSelected="1" topLeftCell="A313" workbookViewId="0">
+      <selection activeCell="A337" sqref="A337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -429,327 +429,327 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>3176652286</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>3173506184</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>3172486789</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>3173809096</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>3123144985</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>3174466432</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>3247439861</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>3104023154</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>3215996243</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>3164602900</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>3176652286</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>3173506184</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>3172486789</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>3173809096</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>3123144985</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>3174466432</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>3247439861</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>3104023154</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>3164602900</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>3176652286</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>3173506184</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>3172486789</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>3173809096</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>3123144985</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>3174466432</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>3247439861</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>3104023154</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>3215996243</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>3164602900</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>3176652286</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>3173506184</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>3172486789</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>3173809096</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>3123144985</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>3174466432</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>3247439861</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>3104023154</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>3215996243</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>3164602900</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>3176652286</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>3173506184</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>3172486789</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>3173809096</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>3123144985</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>3174466432</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>3247439861</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>3215996243</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>3164602900</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>3176652286</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>3173506184</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>3172486789</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>3173809096</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>3123144985</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>3247439861</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>3104023154</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>3215996243</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>3164602900</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>3176652286</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>3173506184</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>3172486789</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>3173809096</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>3123144985</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
@@ -779,327 +779,327 @@
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>3176652286</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>3173506184</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>3172486789</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>3173809096</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>3123144985</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>3174466432</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>3247439861</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>3104023154</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>3215996243</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>3164602900</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>3176652286</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>3173506184</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>3172486789</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>3173809096</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>3123144985</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>3174466432</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>3247439861</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>3104023154</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>3164602900</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>3176652286</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>3173506184</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>3172486789</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>3173809096</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>3123144985</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>3174466432</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>3247439861</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>3104023154</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>3215996243</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>3164602900</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>3176652286</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>3173506184</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>3172486789</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>3173809096</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>3123144985</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>3174466432</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>3247439861</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>3104023154</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>3215996243</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>3164602900</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>3176652286</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>3173506184</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>3172486789</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>3173809096</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>3123144985</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>3174466432</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>3247439861</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>3215996243</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>3164602900</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>3176652286</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>3173506184</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>3172486789</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>3173809096</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>3123144985</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132">
-        <v>3247439861</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133">
-        <v>3104023154</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134">
-        <v>3215996243</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135">
-        <v>3164602900</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136">
-        <v>3176652286</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137">
-        <v>3173506184</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138">
-        <v>3172486789</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139">
-        <v>3173809096</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140">
-        <v>3123144985</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
@@ -1129,327 +1129,327 @@
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146">
-        <v>3176652286</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147">
-        <v>3173506184</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148">
-        <v>3172486789</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149">
-        <v>3173809096</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150">
-        <v>3123144985</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151">
-        <v>3174466432</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152">
-        <v>3247439861</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153">
-        <v>3104023154</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154">
-        <v>3215996243</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155">
-        <v>3164602900</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156">
-        <v>3176652286</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157">
-        <v>3173506184</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158">
-        <v>3172486789</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159">
-        <v>3173809096</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160">
-        <v>3123144985</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161">
-        <v>3174466432</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162">
-        <v>3247439861</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163">
-        <v>3104023154</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165">
-        <v>3164602900</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166">
-        <v>3176652286</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167">
-        <v>3173506184</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168">
-        <v>3172486789</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169">
-        <v>3173809096</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170">
-        <v>3123144985</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171">
-        <v>3174466432</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172">
-        <v>3247439861</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173">
-        <v>3104023154</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174">
-        <v>3215996243</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175">
-        <v>3164602900</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176">
-        <v>3176652286</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177">
-        <v>3173506184</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178">
-        <v>3172486789</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179">
-        <v>3173809096</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180">
-        <v>3123144985</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181">
-        <v>3174466432</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182">
-        <v>3247439861</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183">
-        <v>3104023154</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184">
-        <v>3215996243</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185">
-        <v>3164602900</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186">
-        <v>3176652286</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187">
-        <v>3173506184</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188">
-        <v>3172486789</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189">
-        <v>3173809096</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190">
-        <v>3123144985</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191">
-        <v>3174466432</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192">
-        <v>3247439861</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194">
-        <v>3215996243</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195">
-        <v>3164602900</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196">
-        <v>3176652286</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197">
-        <v>3173506184</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198">
-        <v>3172486789</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199">
-        <v>3173809096</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200">
-        <v>3123144985</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202">
-        <v>3247439861</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203">
-        <v>3104023154</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204">
-        <v>3215996243</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205">
-        <v>3164602900</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206">
-        <v>3176652286</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207">
-        <v>3173506184</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208">
-        <v>3172486789</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209">
-        <v>3173809096</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A210">
-        <v>3123144985</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.3">
@@ -1479,327 +1479,327 @@
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216">
-        <v>3176652286</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217">
-        <v>3173506184</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218">
-        <v>3172486789</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219">
-        <v>3173809096</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220">
-        <v>3123144985</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221">
-        <v>3174466432</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A222">
-        <v>3247439861</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223">
-        <v>3104023154</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A224">
-        <v>3215996243</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225">
-        <v>3164602900</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226">
-        <v>3176652286</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227">
-        <v>3173506184</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228">
-        <v>3172486789</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229">
-        <v>3173809096</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230">
-        <v>3123144985</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A231">
-        <v>3174466432</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232">
-        <v>3247439861</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A233">
-        <v>3104023154</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235">
-        <v>3164602900</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236">
-        <v>3176652286</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A237">
-        <v>3173506184</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238">
-        <v>3172486789</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A239">
-        <v>3173809096</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A240">
-        <v>3123144985</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A241">
-        <v>3174466432</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A242">
-        <v>3247439861</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A243">
-        <v>3104023154</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A244">
-        <v>3215996243</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245">
-        <v>3164602900</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246">
-        <v>3176652286</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A247">
-        <v>3173506184</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A248">
-        <v>3172486789</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A249">
-        <v>3173809096</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250">
-        <v>3123144985</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251">
-        <v>3174466432</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A252">
-        <v>3247439861</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A253">
-        <v>3104023154</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A254">
-        <v>3215996243</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A255">
-        <v>3164602900</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A256">
-        <v>3176652286</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A257">
-        <v>3173506184</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A258">
-        <v>3172486789</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A259">
-        <v>3173809096</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A260">
-        <v>3123144985</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A261">
-        <v>3174466432</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A262">
-        <v>3247439861</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A263">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A264">
-        <v>3215996243</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A265">
-        <v>3164602900</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A266">
-        <v>3176652286</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A267">
-        <v>3173506184</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A268">
-        <v>3172486789</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A269">
-        <v>3173809096</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A270">
-        <v>3123144985</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A271">
-        <v>3174466432</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A272">
-        <v>3247439861</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A273">
-        <v>3104023154</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A274">
-        <v>3215996243</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A275">
-        <v>3164602900</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A276">
-        <v>3176652286</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A277">
-        <v>3173506184</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A278">
-        <v>3172486789</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A279">
-        <v>3173809096</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A280">
-        <v>3123144985</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.3">
@@ -1829,177 +1829,257 @@
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A286">
-        <v>3176652286</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A287">
-        <v>3173506184</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A288">
-        <v>3172486789</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A289">
-        <v>3173809096</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A290">
-        <v>3123144985</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A291">
-        <v>3174466432</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A292">
-        <v>3247439861</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A293">
-        <v>3104023154</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A294">
-        <v>3215996243</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A295">
-        <v>3164602900</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A296">
-        <v>3176652286</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297">
-        <v>3173506184</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A298">
-        <v>3172486789</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A299">
-        <v>3173809096</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A300">
-        <v>3123144985</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A301">
-        <v>3174466432</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A302">
-        <v>3247439861</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A303">
-        <v>3104023154</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A304">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A305">
-        <v>3164602900</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A306">
-        <v>3176652286</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A307">
-        <v>3173506184</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A308">
-        <v>3172486789</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A309">
-        <v>3173809096</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A310">
-        <v>3123144985</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A311">
-        <v>3174466432</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A312">
-        <v>3247439861</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A313">
-        <v>3104023154</v>
+        <v>3164602900</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A314">
-        <v>3215996243</v>
+        <v>3162924200</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A315">
-        <v>3164602900</v>
+        <v>3125278534</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A316">
-        <v>3176652286</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A317">
-        <v>3173506184</v>
+        <v>3247439861</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A318">
-        <v>3172486789</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A319">
-        <v>3173809096</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A320">
-        <v>3123144985</v>
+        <v>3164602900</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A321">
+        <v>3162924200</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A322">
+        <v>3125278534</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A323">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A324">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A325">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A326">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A327">
+        <v>3164602900</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A328">
+        <v>3162924200</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A329">
+        <v>3125278534</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A330">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A331">
+        <v>3247439861</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A332">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A333">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A334">
+        <v>3164602900</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A335">
+        <v>3162924200</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A336">
+        <v>3125278534</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final Funcionando Sin Grupos
</commit_message>
<xml_diff>
--- a/pruebas.xlsx
+++ b/pruebas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\MGS_Selenium\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farud\OneDrive\Escritorio\MGS_Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8302923F-E259-4E9F-8DD3-3CE78FA83AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACF66B5-3678-473B-98CE-49AD0C659047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A512"/>
+  <dimension ref="A1:A750"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A493" workbookViewId="0">
-      <selection activeCell="C505" sqref="C505"/>
+    <sheetView tabSelected="1" topLeftCell="A735" workbookViewId="0">
+      <selection activeCell="C747" sqref="C747"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -409,7 +409,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -419,7 +419,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
@@ -429,7 +429,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
@@ -439,7 +439,7 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
@@ -449,7 +449,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
@@ -459,7 +459,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
@@ -469,7 +469,7 @@
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
@@ -479,7 +479,7 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
@@ -489,7 +489,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
@@ -499,7 +499,7 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
@@ -509,7 +509,7 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
@@ -519,7 +519,7 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
@@ -529,7 +529,7 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
@@ -539,7 +539,7 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
@@ -549,7 +549,7 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
@@ -559,7 +559,7 @@
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
@@ -569,7 +569,7 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
@@ -579,7 +579,7 @@
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
@@ -589,7 +589,7 @@
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
@@ -599,7 +599,7 @@
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
@@ -609,7 +609,7 @@
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
@@ -619,7 +619,7 @@
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
@@ -629,7 +629,7 @@
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
@@ -639,7 +639,7 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
@@ -649,7 +649,7 @@
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
@@ -659,7 +659,7 @@
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
@@ -669,7 +669,7 @@
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
@@ -679,7 +679,7 @@
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
@@ -689,7 +689,7 @@
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
@@ -699,7 +699,7 @@
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
@@ -709,7 +709,7 @@
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
@@ -719,7 +719,7 @@
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
@@ -729,7 +729,7 @@
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
@@ -739,7 +739,7 @@
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
@@ -749,7 +749,7 @@
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
@@ -759,7 +759,7 @@
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
@@ -769,7 +769,7 @@
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
@@ -779,7 +779,7 @@
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
@@ -789,7 +789,7 @@
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
@@ -799,7 +799,7 @@
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
@@ -809,7 +809,7 @@
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
@@ -819,7 +819,7 @@
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
@@ -829,7 +829,7 @@
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
@@ -839,7 +839,7 @@
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
@@ -849,7 +849,7 @@
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
@@ -859,7 +859,7 @@
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
@@ -869,7 +869,7 @@
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
@@ -879,7 +879,7 @@
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
@@ -889,7 +889,7 @@
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
@@ -899,7 +899,7 @@
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
@@ -909,7 +909,7 @@
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
@@ -919,7 +919,7 @@
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
@@ -929,7 +929,7 @@
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
@@ -939,7 +939,7 @@
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
@@ -949,7 +949,7 @@
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
@@ -959,7 +959,7 @@
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
@@ -969,7 +969,7 @@
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
@@ -979,7 +979,7 @@
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
@@ -989,7 +989,7 @@
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
@@ -999,7 +999,7 @@
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
@@ -1009,7 +1009,7 @@
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
@@ -1019,7 +1019,7 @@
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
@@ -1029,7 +1029,7 @@
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
@@ -1039,7 +1039,7 @@
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
@@ -1049,7 +1049,7 @@
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
@@ -1059,7 +1059,7 @@
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
@@ -1069,7 +1069,7 @@
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
@@ -1079,7 +1079,7 @@
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
@@ -1089,7 +1089,7 @@
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
@@ -1099,7 +1099,7 @@
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
@@ -1109,7 +1109,7 @@
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
@@ -1119,7 +1119,7 @@
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
@@ -1129,7 +1129,7 @@
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
@@ -1139,7 +1139,7 @@
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
@@ -1149,7 +1149,7 @@
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
@@ -1159,7 +1159,7 @@
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.3">
@@ -1169,7 +1169,7 @@
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
@@ -1179,7 +1179,7 @@
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.3">
@@ -1189,7 +1189,7 @@
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.3">
@@ -1199,7 +1199,7 @@
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.3">
@@ -1209,7 +1209,7 @@
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.3">
@@ -1219,7 +1219,7 @@
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.3">
@@ -1229,7 +1229,7 @@
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.3">
@@ -1239,7 +1239,7 @@
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.3">
@@ -1249,7 +1249,7 @@
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.3">
@@ -1259,7 +1259,7 @@
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.3">
@@ -1269,7 +1269,7 @@
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.3">
@@ -1279,7 +1279,7 @@
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.3">
@@ -1289,7 +1289,7 @@
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.3">
@@ -1299,7 +1299,7 @@
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.3">
@@ -1309,7 +1309,7 @@
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.3">
@@ -1319,7 +1319,7 @@
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.3">
@@ -1329,7 +1329,7 @@
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.3">
@@ -1339,7 +1339,7 @@
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.3">
@@ -1349,7 +1349,7 @@
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.3">
@@ -1359,7 +1359,7 @@
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
@@ -1369,7 +1369,7 @@
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
@@ -1379,7 +1379,7 @@
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.3">
@@ -1389,7 +1389,7 @@
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.3">
@@ -1399,7 +1399,7 @@
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.3">
@@ -1409,7 +1409,7 @@
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.3">
@@ -1419,7 +1419,7 @@
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.3">
@@ -1429,7 +1429,7 @@
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.3">
@@ -1439,7 +1439,7 @@
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.3">
@@ -1449,7 +1449,7 @@
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A210">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.3">
@@ -1459,7 +1459,7 @@
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A212">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.3">
@@ -1469,7 +1469,7 @@
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.3">
@@ -1479,7 +1479,7 @@
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.3">
@@ -1489,7 +1489,7 @@
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.3">
@@ -1499,7 +1499,7 @@
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.3">
@@ -1509,7 +1509,7 @@
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A222">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.3">
@@ -1519,7 +1519,7 @@
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A224">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.3">
@@ -1529,7 +1529,7 @@
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.3">
@@ -1539,7 +1539,7 @@
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.3">
@@ -1549,7 +1549,7 @@
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.3">
@@ -1559,7 +1559,7 @@
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.3">
@@ -1569,7 +1569,7 @@
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.3">
@@ -1579,7 +1579,7 @@
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.3">
@@ -1589,7 +1589,7 @@
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.3">
@@ -1599,7 +1599,7 @@
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A240">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.3">
@@ -1609,7 +1609,7 @@
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A242">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.3">
@@ -1619,7 +1619,7 @@
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A244">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.3">
@@ -1629,7 +1629,7 @@
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.3">
@@ -1639,7 +1639,7 @@
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A248">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.3">
@@ -1649,12 +1649,12 @@
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250">
-        <v>3104023154</v>
+        <v>3215996243</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.3">
@@ -1664,7 +1664,7 @@
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A253">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.3">
@@ -1674,7 +1674,7 @@
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A255">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.3">
@@ -1684,7 +1684,7 @@
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A257">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.3">
@@ -1694,7 +1694,7 @@
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A259">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.3">
@@ -1704,7 +1704,7 @@
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A261">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.3">
@@ -1714,7 +1714,7 @@
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A263">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.3">
@@ -1724,7 +1724,7 @@
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A265">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.3">
@@ -1734,7 +1734,7 @@
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A267">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.3">
@@ -1744,7 +1744,7 @@
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A269">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.3">
@@ -1754,7 +1754,7 @@
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A271">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.3">
@@ -1764,7 +1764,7 @@
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A273">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.3">
@@ -1774,7 +1774,7 @@
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A275">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.3">
@@ -1784,7 +1784,7 @@
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A277">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.3">
@@ -1794,7 +1794,7 @@
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A279">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.3">
@@ -1804,7 +1804,7 @@
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A281">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.3">
@@ -1814,7 +1814,7 @@
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A283">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.3">
@@ -1824,7 +1824,7 @@
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A285">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.3">
@@ -1834,7 +1834,7 @@
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A287">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.3">
@@ -1844,7 +1844,7 @@
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A289">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.3">
@@ -1854,7 +1854,7 @@
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A291">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.3">
@@ -1864,7 +1864,7 @@
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A293">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.3">
@@ -1874,7 +1874,7 @@
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A295">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.3">
@@ -1884,7 +1884,7 @@
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.3">
@@ -1894,7 +1894,7 @@
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A299">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.3">
@@ -1904,7 +1904,7 @@
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A301">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.3">
@@ -1914,7 +1914,7 @@
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A303">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.3">
@@ -1924,7 +1924,7 @@
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A305">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.3">
@@ -1934,7 +1934,7 @@
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A307">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.3">
@@ -1944,7 +1944,7 @@
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A309">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.3">
@@ -1954,7 +1954,7 @@
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A311">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.3">
@@ -1964,7 +1964,7 @@
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A313">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.3">
@@ -1974,7 +1974,7 @@
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A315">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.3">
@@ -1984,7 +1984,7 @@
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A317">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.3">
@@ -1994,7 +1994,7 @@
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A319">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.3">
@@ -2004,7 +2004,7 @@
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A321">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.3">
@@ -2014,7 +2014,7 @@
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A323">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.3">
@@ -2024,7 +2024,7 @@
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A325">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.3">
@@ -2034,7 +2034,7 @@
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A327">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.3">
@@ -2044,7 +2044,7 @@
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A329">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.3">
@@ -2054,7 +2054,7 @@
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A331">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.3">
@@ -2064,7 +2064,7 @@
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A333">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.3">
@@ -2074,7 +2074,7 @@
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A335">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.3">
@@ -2084,7 +2084,7 @@
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A337">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.3">
@@ -2094,7 +2094,7 @@
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A339">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.3">
@@ -2104,7 +2104,7 @@
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A341">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.3">
@@ -2114,7 +2114,7 @@
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A343">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.3">
@@ -2124,7 +2124,7 @@
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A345">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.3">
@@ -2134,7 +2134,7 @@
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A347">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.3">
@@ -2144,7 +2144,7 @@
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A349">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.3">
@@ -2154,7 +2154,7 @@
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A351">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.3">
@@ -2164,7 +2164,7 @@
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A353">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.3">
@@ -2174,7 +2174,7 @@
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A355">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.3">
@@ -2184,7 +2184,7 @@
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A357">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.3">
@@ -2194,7 +2194,7 @@
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A359">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.3">
@@ -2204,7 +2204,7 @@
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A361">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.3">
@@ -2214,7 +2214,7 @@
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A363">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.3">
@@ -2224,7 +2224,7 @@
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A365">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.3">
@@ -2234,7 +2234,7 @@
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A367">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.3">
@@ -2244,7 +2244,7 @@
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A369">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.3">
@@ -2254,7 +2254,7 @@
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A371">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.3">
@@ -2264,7 +2264,7 @@
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A373">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.3">
@@ -2274,7 +2274,7 @@
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A375">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.3">
@@ -2284,7 +2284,7 @@
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A377">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.3">
@@ -2294,7 +2294,7 @@
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A379">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.3">
@@ -2304,7 +2304,7 @@
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A381">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.3">
@@ -2314,7 +2314,7 @@
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A383">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.3">
@@ -2324,7 +2324,7 @@
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A385">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.3">
@@ -2334,7 +2334,7 @@
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A387">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.3">
@@ -2344,7 +2344,7 @@
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A389">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.3">
@@ -2354,7 +2354,7 @@
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A391">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.3">
@@ -2364,7 +2364,7 @@
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A393">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.3">
@@ -2374,7 +2374,7 @@
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A395">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.3">
@@ -2384,7 +2384,7 @@
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A397">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.3">
@@ -2394,7 +2394,7 @@
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A399">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.3">
@@ -2404,7 +2404,7 @@
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A401">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.3">
@@ -2414,7 +2414,7 @@
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A403">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.3">
@@ -2424,7 +2424,7 @@
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A405">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.3">
@@ -2434,7 +2434,7 @@
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A407">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.3">
@@ -2444,7 +2444,7 @@
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A409">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.3">
@@ -2454,7 +2454,7 @@
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A411">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.3">
@@ -2464,7 +2464,7 @@
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A413">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.3">
@@ -2474,7 +2474,7 @@
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A415">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.3">
@@ -2484,7 +2484,7 @@
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A417">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.3">
@@ -2494,7 +2494,7 @@
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A419">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.3">
@@ -2504,7 +2504,7 @@
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A421">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.3">
@@ -2514,7 +2514,7 @@
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A423">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.3">
@@ -2524,7 +2524,7 @@
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A425">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.3">
@@ -2534,7 +2534,7 @@
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A427">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.3">
@@ -2544,7 +2544,7 @@
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A429">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.3">
@@ -2554,7 +2554,7 @@
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A431">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.3">
@@ -2564,7 +2564,7 @@
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A433">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.3">
@@ -2574,7 +2574,7 @@
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A435">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.3">
@@ -2584,7 +2584,7 @@
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A437">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.3">
@@ -2594,7 +2594,7 @@
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A439">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.3">
@@ -2604,7 +2604,7 @@
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A441">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.3">
@@ -2614,7 +2614,7 @@
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A443">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.3">
@@ -2624,7 +2624,7 @@
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A445">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.3">
@@ -2634,7 +2634,7 @@
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A447">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.3">
@@ -2644,7 +2644,7 @@
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A449">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.3">
@@ -2654,7 +2654,7 @@
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A451">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.3">
@@ -2664,7 +2664,7 @@
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A453">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.3">
@@ -2674,7 +2674,7 @@
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A455">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.3">
@@ -2684,7 +2684,7 @@
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A457">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.3">
@@ -2694,7 +2694,7 @@
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A459">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.3">
@@ -2704,7 +2704,7 @@
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A461">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.3">
@@ -2714,7 +2714,7 @@
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A463">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.3">
@@ -2724,7 +2724,7 @@
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A465">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.3">
@@ -2734,7 +2734,7 @@
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A467">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.3">
@@ -2744,7 +2744,7 @@
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A469">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.3">
@@ -2754,7 +2754,7 @@
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A471">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.3">
@@ -2764,7 +2764,7 @@
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A473">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.3">
@@ -2774,7 +2774,7 @@
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A475">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.3">
@@ -2784,7 +2784,7 @@
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A477">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="478" spans="1:1" x14ac:dyDescent="0.3">
@@ -2794,7 +2794,7 @@
     </row>
     <row r="479" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A479">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.3">
@@ -2804,7 +2804,7 @@
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A481">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.3">
@@ -2814,7 +2814,7 @@
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A483">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.3">
@@ -2824,7 +2824,7 @@
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A485">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.3">
@@ -2834,7 +2834,7 @@
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A487">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.3">
@@ -2844,7 +2844,7 @@
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A489">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.3">
@@ -2854,7 +2854,7 @@
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A491">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.3">
@@ -2864,7 +2864,7 @@
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A493">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.3">
@@ -2874,7 +2874,7 @@
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A495">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.3">
@@ -2884,7 +2884,7 @@
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A497">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.3">
@@ -2894,7 +2894,7 @@
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A499">
-        <v>3215996243</v>
+        <v>3104023154</v>
       </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.3">
@@ -2904,62 +2904,1252 @@
     </row>
     <row r="501" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A501">
-        <v>3215996243</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="502" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A502">
-        <v>3104023154</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="503" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A503">
-        <v>3215996243</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="504" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A504">
-        <v>3104023154</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="505" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A505">
-        <v>3215996243</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="506" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A506">
-        <v>3104023154</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="507" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A507">
-        <v>3215996243</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="508" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A508">
-        <v>3104023154</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="509" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A509">
-        <v>3215996243</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="510" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A510">
-        <v>3104023154</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="511" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A511">
-        <v>3215996243</v>
+        <v>3174466432</v>
       </c>
     </row>
     <row r="512" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A512">
-        <v>3104023154</v>
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A513">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A514">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A515">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A516">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A517">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A518">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A519">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A520">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A521">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A522">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A523">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A524">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A525">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A526">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A527">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A528">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A529">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="530" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A530">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="531" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A531">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A532">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A533">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="534" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A534">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A535">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="536" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A536">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A537">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="538" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A538">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A539">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A540">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A541">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="542" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A542">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="543" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A543">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="544" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A544">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="545" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A545">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="546" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A546">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="547" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A547">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="548" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A548">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="549" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A549">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="550" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A550">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="551" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A551">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="552" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A552">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="553" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A553">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="554" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A554">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="555" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A555">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="556" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A556">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="557" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A557">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="558" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A558">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="559" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A559">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="560" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A560">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="561" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A561">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="562" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A562">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="563" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A563">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="564" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A564">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="565" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A565">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="566" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A566">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="567" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A567">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="568" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A568">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="569" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A569">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="570" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A570">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="571" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A571">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="572" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A572">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="573" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A573">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="574" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A574">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="575" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A575">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="576" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A576">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="577" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A577">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="578" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A578">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="579" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A579">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="580" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A580">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="581" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A581">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="582" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A582">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="583" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A583">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="584" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A584">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="585" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A585">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="586" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A586">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="587" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A587">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="588" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A588">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="589" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A589">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="590" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A590">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="591" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A591">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="592" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A592">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="593" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A593">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="594" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A594">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="595" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A595">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="596" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A596">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="597" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A597">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="598" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A598">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="599" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A599">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="600" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A600">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="601" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A601">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="602" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A602">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="603" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A603">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="604" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A604">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="605" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A605">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="606" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A606">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="607" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A607">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="608" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A608">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="609" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A609">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="610" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A610">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="611" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A611">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="612" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A612">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="613" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A613">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="614" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A614">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="615" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A615">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="616" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A616">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="617" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A617">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="618" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A618">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="619" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A619">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="620" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A620">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="621" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A621">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="622" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A622">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="623" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A623">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="624" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A624">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="625" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A625">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="626" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A626">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="627" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A627">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="628" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A628">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="629" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A629">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="630" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A630">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="631" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A631">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="632" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A632">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="633" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A633">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="634" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A634">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="635" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A635">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="636" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A636">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="637" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A637">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="638" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A638">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="639" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A639">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="640" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A640">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="641" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A641">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="642" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A642">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="643" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A643">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="644" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A644">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="645" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A645">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="646" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A646">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="647" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A647">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="648" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A648">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="649" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A649">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="650" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A650">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="651" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A651">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="652" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A652">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="653" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A653">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="654" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A654">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="655" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A655">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="656" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A656">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="657" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A657">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="658" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A658">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="659" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A659">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="660" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A660">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="661" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A661">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="662" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A662">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="663" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A663">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="664" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A664">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="665" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A665">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="666" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A666">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="667" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A667">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="668" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A668">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="669" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A669">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="670" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A670">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="671" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A671">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="672" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A672">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="673" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A673">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="674" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A674">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="675" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A675">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="676" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A676">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="677" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A677">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="678" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A678">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="679" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A679">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="680" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A680">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="681" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A681">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="682" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A682">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="683" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A683">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="684" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A684">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="685" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A685">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="686" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A686">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="687" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A687">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="688" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A688">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="689" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A689">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="690" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A690">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="691" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A691">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="692" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A692">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="693" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A693">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="694" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A694">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="695" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A695">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="696" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A696">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="697" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A697">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="698" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A698">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="699" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A699">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="700" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A700">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="701" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A701">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="702" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A702">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="703" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A703">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="704" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A704">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="705" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A705">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="706" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A706">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="707" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A707">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="708" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A708">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="709" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A709">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="710" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A710">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="711" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A711">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="712" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A712">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="713" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A713">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="714" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A714">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="715" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A715">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="716" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A716">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="717" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A717">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="718" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A718">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="719" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A719">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="720" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A720">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="721" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A721">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="722" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A722">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="723" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A723">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="724" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A724">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="725" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A725">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="726" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A726">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="727" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A727">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="728" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A728">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="729" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A729">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="730" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A730">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="731" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A731">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="732" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A732">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="733" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A733">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="734" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A734">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="735" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A735">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="736" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A736">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="737" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A737">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="738" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A738">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="739" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A739">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="740" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A740">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="741" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A741">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="742" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A742">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="743" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A743">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="744" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A744">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="745" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A745">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="746" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A746">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="747" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A747">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="748" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A748">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="749" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A749">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="750" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A750">
+        <v>3174466432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final Con Grupos y errores
</commit_message>
<xml_diff>
--- a/pruebas.xlsx
+++ b/pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farud\OneDrive\Escritorio\MGS_Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACF66B5-3678-473B-98CE-49AD0C659047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD07EF46-F7C5-4E11-AE12-0392C5BAA769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A750"/>
+  <dimension ref="A1:A1500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A735" workbookViewId="0">
-      <selection activeCell="C747" sqref="C747"/>
+    <sheetView tabSelected="1" topLeftCell="A1477" workbookViewId="0">
+      <selection activeCell="D1485" sqref="D1485"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4152,6 +4152,3756 @@
         <v>3174466432</v>
       </c>
     </row>
+    <row r="751" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A751">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="752" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A752">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="753" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A753">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="754" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A754">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="755" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A755">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="756" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A756">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="757" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A757">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="758" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A758">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="759" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A759">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="760" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A760">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="761" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A761">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="762" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A762">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="763" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A763">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="764" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A764">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="765" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A765">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="766" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A766">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="767" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A767">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="768" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A768">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="769" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A769">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="770" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A770">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="771" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A771">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="772" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A772">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="773" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A773">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="774" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A774">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="775" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A775">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="776" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A776">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="777" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A777">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="778" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A778">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="779" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A779">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="780" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A780">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="781" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A781">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="782" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A782">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="783" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A783">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="784" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A784">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="785" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A785">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="786" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A786">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="787" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A787">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="788" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A788">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="789" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A789">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="790" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A790">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="791" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A791">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="792" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A792">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="793" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A793">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="794" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A794">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="795" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A795">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="796" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A796">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="797" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A797">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="798" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A798">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="799" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A799">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="800" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A800">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="801" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A801">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="802" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A802">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="803" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A803">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="804" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A804">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="805" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A805">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="806" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A806">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="807" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A807">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="808" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A808">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="809" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A809">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="810" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A810">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="811" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A811">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="812" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A812">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="813" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A813">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="814" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A814">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="815" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A815">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="816" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A816">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="817" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A817">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="818" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A818">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="819" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A819">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="820" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A820">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="821" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A821">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="822" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A822">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="823" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A823">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="824" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A824">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="825" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A825">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="826" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A826">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="827" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A827">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="828" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A828">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="829" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A829">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="830" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A830">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="831" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A831">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="832" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A832">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="833" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A833">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="834" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A834">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="835" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A835">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="836" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A836">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="837" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A837">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="838" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A838">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="839" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A839">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="840" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A840">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="841" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A841">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="842" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A842">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="843" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A843">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="844" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A844">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="845" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A845">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="846" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A846">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="847" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A847">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="848" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A848">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="849" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A849">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="850" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A850">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="851" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A851">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="852" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A852">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="853" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A853">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="854" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A854">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="855" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A855">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="856" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A856">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="857" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A857">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="858" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A858">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="859" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A859">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="860" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A860">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="861" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A861">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="862" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A862">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="863" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A863">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="864" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A864">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="865" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A865">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="866" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A866">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="867" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A867">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="868" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A868">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="869" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A869">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="870" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A870">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="871" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A871">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="872" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A872">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="873" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A873">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="874" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A874">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="875" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A875">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="876" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A876">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="877" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A877">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="878" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A878">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="879" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A879">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="880" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A880">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="881" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A881">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="882" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A882">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="883" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A883">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="884" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A884">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="885" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A885">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="886" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A886">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="887" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A887">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="888" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A888">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="889" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A889">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="890" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A890">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="891" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A891">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="892" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A892">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="893" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A893">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="894" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A894">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="895" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A895">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="896" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A896">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="897" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A897">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="898" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A898">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="899" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A899">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="900" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A900">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="901" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A901">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="902" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A902">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="903" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A903">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="904" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A904">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="905" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A905">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="906" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A906">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="907" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A907">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="908" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A908">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="909" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A909">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="910" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A910">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="911" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A911">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="912" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A912">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="913" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A913">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="914" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A914">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="915" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A915">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="916" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A916">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="917" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A917">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="918" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A918">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="919" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A919">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="920" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A920">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="921" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A921">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="922" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A922">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="923" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A923">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="924" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A924">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="925" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A925">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="926" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A926">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="927" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A927">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="928" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A928">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="929" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A929">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="930" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A930">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="931" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A931">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="932" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A932">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="933" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A933">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="934" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A934">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="935" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A935">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="936" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A936">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="937" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A937">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="938" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A938">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="939" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A939">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="940" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A940">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="941" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A941">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="942" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A942">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="943" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A943">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="944" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A944">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="945" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A945">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="946" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A946">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="947" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A947">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="948" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A948">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="949" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A949">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="950" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A950">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="951" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A951">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="952" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A952">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="953" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A953">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="954" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A954">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="955" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A955">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="956" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A956">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="957" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A957">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="958" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A958">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="959" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A959">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="960" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A960">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="961" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A961">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="962" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A962">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="963" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A963">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="964" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A964">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="965" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A965">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="966" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A966">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="967" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A967">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="968" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A968">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="969" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A969">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="970" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A970">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="971" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A971">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="972" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A972">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="973" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A973">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="974" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A974">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="975" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A975">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="976" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A976">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="977" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A977">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="978" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A978">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="979" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A979">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="980" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A980">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="981" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A981">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="982" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A982">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="983" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A983">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="984" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A984">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="985" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A985">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="986" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A986">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="987" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A987">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="988" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A988">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="989" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A989">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="990" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A990">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="991" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A991">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="992" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A992">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="993" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A993">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="994" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A994">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="995" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A995">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="996" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A996">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="997" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A997">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="998" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A998">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="999" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A999">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1000">
+        <v>3215996243</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1001">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1002">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1003">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1004">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1005">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1006">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1007">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1008">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1009">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1010">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1011">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1012">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1013">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1014">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1015">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1016">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1017">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1018">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1019">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1020">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1021">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1022">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1023">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1024">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1025">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1026">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1027">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1028">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1029">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1030">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1031">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1032">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1033">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1034">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1035">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1036">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1037">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1038">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1039">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1040">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1041">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1042">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1043">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1044">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1045">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1046">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1047">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1048">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1049">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1050">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1051">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1052">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1053">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1054">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1055">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1056">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1057">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1058">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1059">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1060">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1061">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1062">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1063">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1064">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1065">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1066">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1067">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1068">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1069">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1070">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1071">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1072">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1073">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1074">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1075">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1076">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1077">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1078">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1079">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1080">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1081">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1082">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1083">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1084">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1085">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1086">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1087">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1088">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1089">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1090">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1091">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1092">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1093">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1094">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1095">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1096">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1097">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1098">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1099">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1100">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1101">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1102">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1103">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1104">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1105">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1106">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1107">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1108">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1109">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1110">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1111">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1112">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1113">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1114">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1115">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1116">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1117">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1118">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1119">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1120">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1121">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1122">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1123">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1124">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1125">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1126">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1127">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1128">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1129">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1130">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1131">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1132">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1133">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1134">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1135">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1136">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1137">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1138">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1139">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1140">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1141">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1142">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1143">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1144">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1145">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1146">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1147">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1148">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1149">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1150">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1151">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1152">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1153">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1154">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1155">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1156">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1157">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1158">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1159">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1160">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1161">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1162">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1163">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1164">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1165">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1166">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1167">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1168">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1169">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1170">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1171">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1172">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1173">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1174">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1175">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1176">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1177">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1178">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1179">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1180">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1181">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1182">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1183">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1184">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1185">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1186">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1187">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1188">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1189">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1190">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1191">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1192">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1193">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1194">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1195">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1196">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1197">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1198">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1199">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1200">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1201">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1202">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1203">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1204">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1205">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1206">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1207">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1208">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1209">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1210">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1211">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1212">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1213" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1213">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1214">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1215">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1216" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1216">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1217">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1218">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1219">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1220">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1221">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1222">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1223">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1224">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1225">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1226">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1227">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1228">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1229">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1230">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1231">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1232">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1233">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1234">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1235">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1236">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1237">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1238">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1239">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1240">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1241">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1242">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1243">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1244">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1245">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1246">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1247">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1248">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1249">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1250">
+        <v>3104023154</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1251">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1252">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1253">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1254">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1255">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1256">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1257">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1258">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1259">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1260">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1261">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1262">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1263">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1264">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1265">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1266">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1267">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1268">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1269">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1270">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1271">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1272">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1273">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1274">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1275">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1276">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1277">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1278">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1279">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1280">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1281">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1282">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1283">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1284">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1285">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1286">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1287">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1288">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1289">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1290">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1291">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1292" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1292">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1293">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1294">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1295">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1296">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1297">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1298">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1299">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1300">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1301">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1302">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1303">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1304">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1305">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1306">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1307">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1308">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1309">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1310">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1311">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1312">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1313">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1314">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1315">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1316">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1317">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1318">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1319">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1320">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1321">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1322">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1323">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1324">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1325">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1326">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1327">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1328">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1329">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1330">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1331">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1332">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1333">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1334">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1335">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1336">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1337">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1338">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1339">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1340">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1341">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1342">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1343">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1344">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1345">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1346">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1347">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1348">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1349">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1350">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1351">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1352">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1353">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1354">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1355">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1356">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1357">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1358" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1358">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1359" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1359">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1360" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1360">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1361">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1362">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1363">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1364">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1365">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1366">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1367">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1368">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1369">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1370">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1371">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1372">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1373" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1373">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1374" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1374">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1375">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1376">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1377">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1378">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1379">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1380">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1381">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1382">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1383">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1384">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1385">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1386">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1387">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1388">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1389">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1390">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1391">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1392">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1393">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1394">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1395">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1396">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1397">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1398">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1399">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1400">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1401">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1402">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1403">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1404">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1405">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1406">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1407">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1408">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1409">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1410">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1411">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1412">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1413">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1414">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1415">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1416">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1417">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1418">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1419">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1420">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1421">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1422">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1423">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1424">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1425">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1426">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1427">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1428">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1429">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1430">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1431">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1432">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1433">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1434">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1435">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1436" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1436">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1437" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1437">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1438">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1439">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1440">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1441">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1442">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1443">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1444">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1445">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1446">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1447">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1448">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1449">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1450">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1451">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1452">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1453" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1453">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1454">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1455">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1456" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1456">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1457">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1458" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1458">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1459" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1459">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1460" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1460">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1461" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1461">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1462" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1462">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1463" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1463">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1464" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1464">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1465" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1465">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1466" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1466">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1467" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1467">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1468" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1468">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1469" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1469">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1470" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1470">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1471" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1471">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1472" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1472">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1473" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1473">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1474" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1474">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1475" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1475">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1476" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1476">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1477" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1477">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1478" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1478">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1479" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1479">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1480" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1480">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1481" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1481">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1482" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1482">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1483">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1484">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1485" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1485">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1486" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1486">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1487" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1487">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1488" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1488">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1489" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1489">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1490" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1490">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1491" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1491">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1492" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1492">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1493" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1493">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1494" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1494">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1495" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1495">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1496" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1496">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1497" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1497">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1498" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1498">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1499" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1499">
+        <v>3174466432</v>
+      </c>
+    </row>
+    <row r="1500" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1500">
+        <v>3174466432</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>